<commit_message>
Push Search Function integrated to backend
</commit_message>
<xml_diff>
--- a/cab_backend/Document Format/MONTHLY CONSUMPTION SECTION.xlsx
+++ b/cab_backend/Document Format/MONTHLY CONSUMPTION SECTION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cabwad\testing\IMS-Cabwad\cab_backend\Document Format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622671BD-5A3B-4752-B514-E88B9A676AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F943006-4CF1-43BC-ADCC-C2A73261CB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,16 +100,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -147,9 +144,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>388718</xdr:colOff>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>95</xdr:rowOff>
+      <xdr:rowOff>29457</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -173,7 +170,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1135478" cy="1097375"/>
+          <a:ext cx="1165860" cy="1126737"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -448,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:G9"/>
+  <dimension ref="A3:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,17 +460,17 @@
     <col min="7" max="8" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C3" s="7" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C4" s="6" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -481,11 +478,38 @@
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G5" s="1"/>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F9" s="4"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>